<commit_message>
fixed no data error, no assortment error, and state warning error
</commit_message>
<xml_diff>
--- a/Projects/MOLSONCOORSCA/Data/Competitive Brands v1.xlsx
+++ b/Projects/MOLSONCOORSCA/Data/Competitive Brands v1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Granular Groups" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,9 +16,11 @@
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Granular Groups link to stores'!$A$2:$K$2</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Granular Groups'!$A$2:$F$152</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Granular Groups'!$A$2:$F$152</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Granular Groups'!$A$2:$F$152</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">'Granular Groups link to stores'!$A$2:$EM$59</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Granular Groups link to stores'!$A$2:$K$2</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Granular Groups link to stores'!$A$2:$K$2</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Granular Groups link to stores'!$A$2:$K$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -212,7 +214,7 @@
     <t xml:space="preserve">ON</t>
   </si>
   <si>
-    <t xml:space="preserve">QB</t>
+    <t xml:space="preserve">QC</t>
   </si>
   <si>
     <t xml:space="preserve">NB</t>
@@ -405,7 +407,7 @@
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="11">
     <dxf>
       <fill>
         <patternFill>
@@ -504,20 +506,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFBE5D6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF4B183"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <colors>
     <indexedColors>
@@ -597,7 +585,7 @@
   </sheetPr>
   <dimension ref="A1:F152"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="D155" activeCellId="0" sqref="D155"/>
@@ -605,13 +593,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="26.3214285714286"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.4183673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="25.9183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3674,17 +3662,17 @@
   </sheetPr>
   <dimension ref="A1:K12"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="11" min="2" style="7" width="20.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="7" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="5" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="2" style="7" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="7" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>